<commit_message>
Recover the coding preparation. Day 1-Array.
</commit_message>
<xml_diff>
--- a/C-Interview/Leetcode/Problem-tracker.xlsx
+++ b/C-Interview/Leetcode/Problem-tracker.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12960"/>
+    <workbookView windowWidth="24750" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,8 @@
     <t>https://leetcode.com/problems/two-sum/description/</t>
   </si>
   <si>
-    <t>2025.2.22; 2025.2.11; 2024.10.31</t>
+    <t>2024.10.31;
+2025.2.22; 2025.2.11; 2025.10.27</t>
   </si>
   <si>
     <t>K Closet Points to Origin</t>
@@ -888,7 +889,8 @@
     <t>https://leetcode.com/problems/best-time-to-buy-and-sell-stock/description/</t>
   </si>
   <si>
-    <t>2025.2.11; 2024.10.31</t>
+    <t>2024.10.31;
+2025.2.11; 2025.10.27</t>
   </si>
   <si>
     <t>Implement Trie (Prefix Tree)</t>
@@ -1060,19 +1062,15 @@
     <t>https://leetcode.com/problems/product-of-array-except-self/description/</t>
   </si>
   <si>
-    <t>2025.2.12; 2024.11.3</t>
+    <t>2024.11.3
+2025.2.12;
+2025.10.27;</t>
   </si>
   <si>
     <t>Maximum Subarray</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Maximum Subarray Sum with </t>
     </r>
     <r>
@@ -1142,7 +1140,8 @@
         <rFont val="Cambria"/>
         <charset val="134"/>
       </rPr>
-      <t>Did not solve second time</t>
+      <t>Did not solve second time
+Did not solve third time</t>
     </r>
   </si>
   <si>
@@ -1200,7 +1199,8 @@
     <t>https://leetcode.com/problems/maximum-subarray/description/</t>
   </si>
   <si>
-    <t>2025.2.12; 2024.11.4</t>
+    <t>2024.11.4
+2025.2.12; 2025.10.27</t>
   </si>
   <si>
     <t>Contains Duplicate</t>
@@ -4683,6 +4683,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <i/>
       <u/>
@@ -4691,14 +4697,8 @@
       <name val="Cambria"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4720,6 +4720,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5051,7 +5057,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5075,16 +5081,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -5093,89 +5099,89 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5231,6 +5237,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5555,20 +5564,20 @@
   <sheetPr/>
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.75" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.6333333333333" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3583333333333" style="10" customWidth="1"/>
+    <col min="1" max="1" width="6.75454545454545" style="11" customWidth="1"/>
+    <col min="2" max="2" width="25.6363636363636" style="10" customWidth="1"/>
+    <col min="3" max="3" width="12.2545454545455" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3545454545455" style="10" customWidth="1"/>
     <col min="5" max="5" width="94.9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.2583333333333" style="10" customWidth="1"/>
+    <col min="6" max="6" width="43.2545454545455" style="10" customWidth="1"/>
     <col min="7" max="7" width="18.3" style="10" customWidth="1"/>
-    <col min="8" max="8" width="32.6666666666667" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.6636363636364" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5598,7 +5607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="85.5" spans="1:8">
+    <row r="2" ht="98" spans="1:8">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -5620,11 +5629,11 @@
       <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" ht="128.25" spans="1:8">
+    <row r="3" ht="126" spans="1:8">
       <c r="A3" s="15">
         <v>973</v>
       </c>
@@ -5686,7 +5695,7 @@
       <c r="G5" s="5"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" ht="85.5" spans="1:8">
+    <row r="6" ht="98" spans="1:8">
       <c r="A6" s="15">
         <v>733</v>
       </c>
@@ -5730,7 +5739,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" ht="85.5" spans="1:8">
+    <row r="8" ht="98" spans="1:8">
       <c r="A8" s="15">
         <v>235</v>
       </c>
@@ -5756,7 +5765,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" ht="85.5" spans="1:8">
+    <row r="9" ht="84" spans="1:8">
       <c r="A9" s="15">
         <v>226</v>
       </c>
@@ -5782,7 +5791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" ht="28" spans="1:8">
       <c r="A10" s="16">
         <v>104</v>
       </c>
@@ -5800,7 +5809,7 @@
       <c r="G10" s="5"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" ht="85.5" spans="1:8">
+    <row r="11" ht="84" spans="1:8">
       <c r="A11" s="15">
         <v>232</v>
       </c>
@@ -5826,7 +5835,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" ht="99.75" spans="1:8">
+    <row r="12" ht="112" spans="1:8">
       <c r="A12" s="15">
         <v>20</v>
       </c>
@@ -5852,7 +5861,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" ht="28" spans="1:8">
       <c r="A13" s="16">
         <v>225</v>
       </c>
@@ -5870,7 +5879,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" ht="71.25" spans="1:8">
+    <row r="14" ht="98" spans="1:8">
       <c r="A14" s="15">
         <v>141</v>
       </c>
@@ -5896,7 +5905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" ht="85.5" spans="1:8">
+    <row r="15" ht="84" spans="1:8">
       <c r="A15" s="15">
         <v>206</v>
       </c>
@@ -5958,7 +5967,7 @@
       <c r="G17" s="5"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" ht="85.5" spans="1:8">
+    <row r="18" ht="84" spans="1:8">
       <c r="A18" s="15">
         <v>33</v>
       </c>
@@ -5984,7 +5993,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" ht="99.75" spans="1:8">
+    <row r="19" ht="112" spans="1:8">
       <c r="A19" s="15">
         <v>704</v>
       </c>
@@ -6064,7 +6073,7 @@
       <c r="G22" s="5"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" ht="99.75" spans="1:8">
+    <row r="23" ht="140" spans="1:8">
       <c r="A23" s="14">
         <v>121</v>
       </c>
@@ -6086,11 +6095,11 @@
       <c r="G23" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="24" ht="85.5" spans="1:8">
+    <row r="24" ht="98" spans="1:8">
       <c r="A24" s="16">
         <v>208</v>
       </c>
@@ -6114,7 +6123,7 @@
       </c>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" ht="114" spans="1:8">
+    <row r="25" ht="126" spans="1:8">
       <c r="A25" s="18">
         <v>238</v>
       </c>
@@ -6136,11 +6145,11 @@
       <c r="G25" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="26" ht="99.75" spans="1:8">
+    <row r="26" ht="98" spans="1:8">
       <c r="A26" s="19">
         <v>53</v>
       </c>
@@ -6162,11 +6171,11 @@
       <c r="G26" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" ht="85.5" spans="1:8">
+    <row r="27" ht="84" spans="1:8">
       <c r="A27" s="14">
         <v>217</v>
       </c>
@@ -6192,7 +6201,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" ht="85.5" spans="1:8">
+    <row r="28" ht="84" spans="1:8">
       <c r="A28" s="16">
         <v>56</v>
       </c>
@@ -6216,8 +6225,8 @@
       </c>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" ht="85.5" spans="1:8">
-      <c r="A29" s="19">
+    <row r="29" ht="112" spans="1:8">
+      <c r="A29" s="20">
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -6240,8 +6249,8 @@
       </c>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" ht="142.5" spans="1:8">
-      <c r="A30" s="19">
+    <row r="30" ht="154" spans="1:8">
+      <c r="A30" s="20">
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -6266,8 +6275,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" ht="128.25" spans="1:8">
-      <c r="A31" s="19">
+    <row r="31" ht="126" spans="1:8">
+      <c r="A31" s="20">
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -6290,11 +6299,11 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" ht="99.75" spans="1:8">
-      <c r="A32" s="20">
+    <row r="32" ht="112" spans="1:8">
+      <c r="A32" s="21">
         <v>70</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="22" t="s">
         <v>153</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -6316,8 +6325,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" ht="114" spans="1:8">
-      <c r="A33" s="19">
+    <row r="33" ht="126" spans="1:8">
+      <c r="A33" s="20">
         <v>322</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -6340,8 +6349,8 @@
       </c>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" ht="156.75" spans="1:8">
-      <c r="A34" s="19">
+    <row r="34" ht="154" spans="1:8">
+      <c r="A34" s="20">
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -6366,8 +6375,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" ht="199.5" spans="1:8">
-      <c r="A35" s="19">
+    <row r="35" ht="196" spans="1:8">
+      <c r="A35" s="20">
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -6392,7 +6401,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" ht="185.25" spans="1:8">
+    <row r="36" ht="182" spans="1:8">
       <c r="A36" s="14">
         <v>242</v>
       </c>
@@ -6418,7 +6427,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" ht="199.5" spans="1:8">
+    <row r="37" ht="196" spans="1:8">
       <c r="A37" s="16">
         <v>198</v>
       </c>
@@ -6444,8 +6453,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" ht="99.75" spans="1:8">
-      <c r="A38" s="19">
+    <row r="38" ht="112" spans="1:8">
+      <c r="A38" s="20">
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -6469,7 +6478,7 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" ht="131" customHeight="1" spans="1:8">
-      <c r="A39" s="19">
+      <c r="A39" s="20">
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -6492,8 +6501,8 @@
       </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" ht="128.25" spans="1:8">
-      <c r="A40" s="19">
+    <row r="40" ht="126" spans="1:8">
+      <c r="A40" s="20">
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -6516,7 +6525,7 @@
       </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" ht="171" spans="1:8">
+    <row r="41" ht="182" spans="1:8">
       <c r="A41" s="14">
         <v>125</v>
       </c>
@@ -6542,8 +6551,8 @@
         <v>208</v>
       </c>
     </row>
-    <row r="42" ht="85.5" spans="1:8">
-      <c r="A42" s="19">
+    <row r="42" ht="98" spans="1:8">
+      <c r="A42" s="20">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -6568,8 +6577,8 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" ht="99.75" spans="1:8">
-      <c r="A43" s="19">
+    <row r="43" ht="112" spans="1:8">
+      <c r="A43" s="20">
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -6592,8 +6601,8 @@
       </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" ht="85.5" spans="1:8">
-      <c r="A44" s="19">
+    <row r="44" ht="98" spans="1:8">
+      <c r="A44" s="20">
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -6617,7 +6626,7 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" ht="208" customHeight="1" spans="1:8">
-      <c r="A45" s="19">
+      <c r="A45" s="20">
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -6642,7 +6651,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="46" ht="85.5" spans="1:8">
+    <row r="46" ht="84" spans="1:8">
       <c r="A46" s="16">
         <v>836</v>
       </c>
@@ -6692,7 +6701,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" ht="85.5" spans="1:8">
+    <row r="48" ht="84" spans="1:8">
       <c r="A48" s="14">
         <v>49</v>
       </c>
@@ -6718,7 +6727,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="49" ht="85.5" spans="1:8">
+    <row r="49" ht="84" spans="1:8">
       <c r="A49" s="18">
         <v>380</v>
       </c>
@@ -6744,7 +6753,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="50" ht="156.75" spans="1:8">
+    <row r="50" ht="182" spans="1:8">
       <c r="A50" s="18">
         <v>41</v>
       </c>
@@ -6770,8 +6779,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="51" ht="156.75" spans="1:8">
-      <c r="A51" s="19">
+    <row r="51" ht="154" spans="1:8">
+      <c r="A51" s="20">
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -6796,8 +6805,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="52" ht="71.25" spans="1:8">
-      <c r="A52" s="19">
+    <row r="52" ht="70" spans="1:8">
+      <c r="A52" s="20">
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -6820,7 +6829,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="53" ht="85.5" spans="1:8">
+    <row r="53" ht="84" spans="1:8">
       <c r="A53" s="16">
         <v>21</v>
       </c>
@@ -6846,8 +6855,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" ht="142.5" spans="1:8">
-      <c r="A54" s="19">
+    <row r="54" ht="140" spans="1:8">
+      <c r="A54" s="20">
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -6870,7 +6879,7 @@
       </c>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" ht="85.5" spans="1:8">
+    <row r="55" ht="84" spans="1:8">
       <c r="A55" s="16">
         <v>278</v>
       </c>
@@ -6894,7 +6903,7 @@
       </c>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" ht="99.75" spans="1:8">
+    <row r="56" ht="98" spans="1:8">
       <c r="A56" s="16">
         <v>409</v>
       </c>
@@ -6918,8 +6927,8 @@
       </c>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" ht="99.75" spans="1:8">
-      <c r="A57" s="19">
+    <row r="57" ht="112" spans="1:8">
+      <c r="A57" s="20">
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -6942,8 +6951,8 @@
       </c>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" ht="99.75" spans="1:8">
-      <c r="A58" s="19">
+    <row r="58" ht="126" spans="1:8">
+      <c r="A58" s="20">
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -6966,8 +6975,8 @@
       </c>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" ht="99.75" spans="1:8">
-      <c r="A59" s="19">
+    <row r="59" ht="112" spans="1:8">
+      <c r="A59" s="20">
         <v>543</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -7009,12 +7018,12 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="195.133333333333" customWidth="1"/>
+    <col min="1" max="1" width="195.136363636364" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:1">
+    <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
         <v>301</v>
       </c>
@@ -7073,12 +7082,12 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="24.1083333333333" customWidth="1"/>
-    <col min="5" max="5" width="63.4416666666667" customWidth="1"/>
+    <col min="2" max="2" width="24.1090909090909" customWidth="1"/>
+    <col min="5" max="5" width="63.4454545454545" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="8" max="8" width="30.225" customWidth="1"/>
+    <col min="8" max="8" width="30.2272727272727" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="141" customHeight="1" spans="1:8">
@@ -7107,7 +7116,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="114" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="126" spans="1:8">
       <c r="A2" s="2">
         <v>733</v>
       </c>
@@ -7133,7 +7142,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="121.5" spans="1:8">
+    <row r="3" s="1" customFormat="1" ht="126" spans="1:8">
       <c r="A3" s="2">
         <v>141</v>
       </c>
@@ -7159,7 +7168,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="121.5" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="126" spans="1:8">
       <c r="A4" s="7">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
Coding recovery. Day 2-String.
</commit_message>
<xml_diff>
--- a/C-Interview/Leetcode/Problem-tracker.xlsx
+++ b/C-Interview/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="308">
   <si>
     <t>No.</t>
   </si>
@@ -1071,6 +1071,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: This problem follows the "Maximum Subarray Sum with </t>
     </r>
     <r>
@@ -2186,6 +2192,10 @@
     <t>https://leetcode.com/problems/valid-anagram/description/</t>
   </si>
   <si>
+    <t>2024.11.11
+2025.2.16; 2025.10.28</t>
+  </si>
+  <si>
     <t>House Robber</t>
   </si>
   <si>
@@ -2568,7 +2578,8 @@
     <t>https://leetcode.com/problems/valid-palindrome/description/</t>
   </si>
   <si>
-    <t>2025.2.20; 2025.11.13</t>
+    <t>2024.11.13
+2025.2.20;  2025.10.28</t>
   </si>
   <si>
     <t>Longest Substring Without Repeating Characters</t>
@@ -2578,12 +2589,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem follows the Sliding Window pattern where we </t>
     </r>
     <r>
@@ -2635,7 +2640,8 @@
       </rPr>
       <t xml:space="preserve">
 Set is used for checking duplicates instantly
-Not solved second time</t>
+Not solved second time
+Not solved thied time</t>
     </r>
   </si>
   <si>
@@ -2693,7 +2699,8 @@
     <t>https://leetcode.com/problems/longest-substring-without-repeating-characters/description/</t>
   </si>
   <si>
-    <t>2025.2.20; 2025.11.17</t>
+    <t>2024.11.17
+2025.2.20; 2025.10.28</t>
   </si>
   <si>
     <t>Pow(x, n)</t>
@@ -4683,18 +4690,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -5564,8 +5571,8 @@
   <sheetPr/>
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -6423,8 +6430,8 @@
       <c r="G36" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>175</v>
+      <c r="H36" s="5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="37" ht="196" spans="1:8">
@@ -6432,25 +6439,25 @@
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>154</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="38" ht="112" spans="1:8">
@@ -6458,22 +6465,22 @@
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H38" s="4"/>
     </row>
@@ -6482,22 +6489,22 @@
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H39" s="4"/>
     </row>
@@ -6506,22 +6513,22 @@
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H40" s="4"/>
     </row>
@@ -6530,51 +6537,51 @@
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H41" s="4" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="42" ht="98" spans="1:8">
+      <c r="H41" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" ht="112" spans="1:8">
       <c r="A42" s="20">
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H42" s="4" t="s">
         <v>214</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="43" ht="112" spans="1:8">
@@ -6582,22 +6589,22 @@
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H43" s="4"/>
     </row>
@@ -6606,22 +6613,22 @@
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="H44" s="4"/>
     </row>
@@ -6630,25 +6637,25 @@
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" ht="84" spans="1:8">
@@ -6656,22 +6663,22 @@
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H46" s="4"/>
     </row>
@@ -6680,25 +6687,25 @@
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" ht="84" spans="1:8">
@@ -6706,25 +6713,25 @@
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" ht="84" spans="1:8">
@@ -6732,7 +6739,7 @@
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -6741,16 +6748,16 @@
         <v>10</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" ht="182" spans="1:8">
@@ -6758,25 +6765,25 @@
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" ht="154" spans="1:8">
@@ -6784,25 +6791,25 @@
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" ht="70" spans="1:8">
@@ -6810,23 +6817,23 @@
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" ht="84" spans="1:8">
@@ -6834,7 +6841,7 @@
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>28</v>
@@ -6843,13 +6850,13 @@
         <v>66</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>28</v>
@@ -6860,22 +6867,22 @@
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="H54" s="4"/>
     </row>
@@ -6884,7 +6891,7 @@
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>65</v>
@@ -6893,13 +6900,13 @@
         <v>89</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -6908,7 +6915,7 @@
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>50</v>
@@ -6917,13 +6924,13 @@
         <v>10</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="H56" s="4"/>
     </row>
@@ -6932,22 +6939,22 @@
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H57" s="4"/>
     </row>
@@ -6956,22 +6963,22 @@
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H58" s="4"/>
     </row>
@@ -6980,22 +6987,22 @@
         <v>543</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="H59" s="4"/>
     </row>
@@ -7025,12 +7032,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
       <c r="A2" s="10" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -7098,7 +7105,7 @@
         <v>153</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>154</v>
@@ -7113,7 +7120,7 @@
         <v>157</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7139,7 +7146,7 @@
         <v>32</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7165,7 +7172,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7191,7 +7198,7 @@
         <v>75</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Hash Table two problems.
</commit_message>
<xml_diff>
--- a/C-Interview/Leetcode/Problem-tracker.xlsx
+++ b/C-Interview/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="11190"/>
+    <workbookView windowWidth="24740" windowHeight="11200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="309">
   <si>
     <t>No.</t>
   </si>
@@ -2589,6 +2589,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Problem Pattern: The problem follows the Sliding Window pattern where we </t>
     </r>
     <r>
@@ -3151,7 +3157,8 @@
     <t>https://leetcode.com/problems/ransom-note/description/</t>
   </si>
   <si>
-    <t>2025.2.22; 2024.11.25</t>
+    <t>2025.2.22; 2024.11.25,
+2025.10.29</t>
   </si>
   <si>
     <t>Group Anagram</t>
@@ -3546,7 +3553,8 @@
     <t>https://leetcode.com/problems/first-missing-positive/description/</t>
   </si>
   <si>
-    <t>2025.2.22; 2024.12.18</t>
+    <t xml:space="preserve"> 2024.12.18
+2025.2.22; 2025.10.29</t>
   </si>
   <si>
     <t>LRU Cache</t>
@@ -3696,16 +3704,20 @@
     <t>https://leetcode.com/problems/lru-cache/description/</t>
   </si>
   <si>
+    <t>2025.2.23; 2024.12.1
+2025.10.29</t>
+  </si>
+  <si>
+    <t>All O`one Data Structure</t>
+  </si>
+  <si>
+    <t>Not Solved in O(1) Time Complexity</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/all-oone-data-structure/description/</t>
+  </si>
+  <si>
     <t>2025.2.23; 2024.12.1</t>
-  </si>
-  <si>
-    <t>All O`one Data Structure</t>
-  </si>
-  <si>
-    <t>Not Solved in O(1) Time Complexity</t>
-  </si>
-  <si>
-    <t>https://leetcode.com/problems/all-oone-data-structure/description/</t>
   </si>
   <si>
     <t>Merge Two Sorted Lists</t>
@@ -4690,18 +4702,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -5571,8 +5583,8 @@
   <sheetPr/>
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -6704,7 +6716,7 @@
       <c r="G47" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="5" t="s">
         <v>242</v>
       </c>
     </row>
@@ -6782,7 +6794,7 @@
       <c r="G50" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="H50" s="4" t="s">
+      <c r="H50" s="5" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6808,7 +6820,7 @@
       <c r="G51" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="H51" s="4" t="s">
+      <c r="H51" s="5" t="s">
         <v>266</v>
       </c>
     </row>
@@ -6833,7 +6845,7 @@
         <v>269</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" ht="84" spans="1:8">
@@ -6841,7 +6853,7 @@
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>28</v>
@@ -6850,13 +6862,13 @@
         <v>66</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>28</v>
@@ -6867,22 +6879,22 @@
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H54" s="4"/>
     </row>
@@ -6891,7 +6903,7 @@
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>65</v>
@@ -6900,13 +6912,13 @@
         <v>89</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -6915,7 +6927,7 @@
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>50</v>
@@ -6924,13 +6936,13 @@
         <v>10</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="H56" s="4"/>
     </row>
@@ -6939,22 +6951,22 @@
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="H57" s="4"/>
     </row>
@@ -6963,22 +6975,22 @@
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>195</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H58" s="4"/>
     </row>
@@ -6987,22 +6999,22 @@
         <v>543</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H59" s="4"/>
     </row>
@@ -7032,12 +7044,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
       <c r="A2" s="10" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -7105,7 +7117,7 @@
         <v>153</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>154</v>
@@ -7120,7 +7132,7 @@
         <v>157</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7146,7 +7158,7 @@
         <v>32</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7172,7 +7184,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7198,7 +7210,7 @@
         <v>75</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coding recovery Day 4-sorting.
</commit_message>
<xml_diff>
--- a/C-Interview/Leetcode/Problem-tracker.xlsx
+++ b/C-Interview/Leetcode/Problem-tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24740" windowHeight="11200"/>
+    <workbookView windowWidth="24750" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -752,7 +752,8 @@
     <t>https://leetcode.com/problems/search-in-rotated-sorted-array/description/</t>
   </si>
   <si>
-    <t>2025.2.13; 2025.1.27; 2024.11.6</t>
+    <t>2025.2.13; 2025.1.27; 2024.11.6
+, 2025.10.30</t>
   </si>
   <si>
     <t>Binary Search</t>
@@ -806,7 +807,7 @@
     <t>https://leetcode.com/problems/binary-search/description/</t>
   </si>
   <si>
-    <t>2025.2.24; 2025.1.26</t>
+    <t>2025.2.24; 2025.1.26, 2025.10.30</t>
   </si>
   <si>
     <t>Subsets</t>
@@ -4702,18 +4703,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -5583,8 +5584,8 @@
   <sheetPr/>
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -6008,7 +6009,7 @@
       <c r="G18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="5" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Coding recovery. Day 5-Recursion.
</commit_message>
<xml_diff>
--- a/C-Interview/Leetcode/Problem-tracker.xlsx
+++ b/C-Interview/Leetcode/Problem-tracker.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="310">
   <si>
     <t>No.</t>
   </si>
@@ -817,6 +817,9 @@
   </si>
   <si>
     <t>Recursion</t>
+  </si>
+  <si>
+    <t>2025.10.31</t>
   </si>
   <si>
     <t>Combination</t>
@@ -5585,7 +5588,7 @@
   <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -6055,17 +6058,19 @@
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="16">
         <v>77</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>97</v>
@@ -6073,17 +6078,19 @@
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="16">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>97</v>
@@ -6091,32 +6098,34 @@
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="23" ht="140" spans="1:8">
       <c r="A23" s="14">
         <v>121</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" ht="98" spans="1:8">
@@ -6124,22 +6133,22 @@
         <v>208</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H24" s="4"/>
     </row>
@@ -6148,25 +6157,25 @@
         <v>238</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" ht="98" spans="1:8">
@@ -6174,25 +6183,25 @@
         <v>53</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" ht="84" spans="1:8">
@@ -6200,25 +6209,25 @@
         <v>217</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" ht="84" spans="1:8">
@@ -6226,22 +6235,22 @@
         <v>56</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H28" s="4"/>
     </row>
@@ -6250,22 +6259,22 @@
         <v>152</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H29" s="4"/>
     </row>
@@ -6274,25 +6283,25 @@
         <v>15</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" ht="126" spans="1:8">
@@ -6300,22 +6309,22 @@
         <v>57</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H31" s="4"/>
     </row>
@@ -6324,25 +6333,25 @@
         <v>70</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" ht="126" spans="1:8">
@@ -6350,22 +6359,22 @@
         <v>322</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H33" s="4"/>
     </row>
@@ -6374,25 +6383,25 @@
         <v>11</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" ht="196" spans="1:8">
@@ -6400,25 +6409,25 @@
         <v>239</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" ht="182" spans="1:8">
@@ -6426,25 +6435,25 @@
         <v>242</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" ht="196" spans="1:8">
@@ -6452,25 +6461,25 @@
         <v>198</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="38" ht="112" spans="1:8">
@@ -6478,22 +6487,22 @@
         <v>300</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H38" s="4"/>
     </row>
@@ -6502,22 +6511,22 @@
         <v>371</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H39" s="4"/>
     </row>
@@ -6526,22 +6535,22 @@
         <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H40" s="4"/>
     </row>
@@ -6550,25 +6559,25 @@
         <v>125</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" ht="112" spans="1:8">
@@ -6576,25 +6585,25 @@
         <v>3</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" ht="112" spans="1:8">
@@ -6602,22 +6611,22 @@
         <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H43" s="4"/>
     </row>
@@ -6626,22 +6635,22 @@
         <v>69</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H44" s="4"/>
     </row>
@@ -6650,25 +6659,25 @@
         <v>424</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="46" ht="84" spans="1:8">
@@ -6676,22 +6685,22 @@
         <v>836</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H46" s="4"/>
     </row>
@@ -6700,25 +6709,25 @@
         <v>383</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" ht="84" spans="1:8">
@@ -6726,25 +6735,25 @@
         <v>49</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" ht="84" spans="1:8">
@@ -6752,7 +6761,7 @@
         <v>380</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -6761,16 +6770,16 @@
         <v>10</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" ht="182" spans="1:8">
@@ -6778,25 +6787,25 @@
         <v>41</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" ht="154" spans="1:8">
@@ -6804,25 +6813,25 @@
         <v>146</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" ht="70" spans="1:8">
@@ -6830,23 +6839,23 @@
         <v>432</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" ht="84" spans="1:8">
@@ -6854,7 +6863,7 @@
         <v>21</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>28</v>
@@ -6863,13 +6872,13 @@
         <v>66</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>28</v>
@@ -6880,22 +6889,22 @@
         <v>110</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H54" s="4"/>
     </row>
@@ -6904,7 +6913,7 @@
         <v>278</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>65</v>
@@ -6913,13 +6922,13 @@
         <v>89</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H55" s="4"/>
     </row>
@@ -6928,7 +6937,7 @@
         <v>409</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>50</v>
@@ -6937,13 +6946,13 @@
         <v>10</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="H56" s="4"/>
     </row>
@@ -6952,22 +6961,22 @@
         <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H57" s="4"/>
     </row>
@@ -6976,22 +6985,22 @@
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="H58" s="4"/>
     </row>
@@ -7000,22 +7009,22 @@
         <v>543</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H59" s="4"/>
     </row>
@@ -7045,12 +7054,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" ht="409" customHeight="1" spans="1:1">
       <c r="A2" s="10" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -7115,25 +7124,25 @@
         <v>70</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7159,7 +7168,7 @@
         <v>32</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7185,7 +7194,7 @@
         <v>69</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="126" spans="1:8">
@@ -7211,7 +7220,7 @@
         <v>75</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>